<commit_message>
change language from lasat year to pervious rotation
</commit_message>
<xml_diff>
--- a/data/risk_index_matrix.xlsx
+++ b/data/risk_index_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox (cesar)\cesar Team Folder\_Customer Project Files\1006 GRDC\1006CR12 RLEM\2. Milestones\14. Seasonal risk forecast\Modelling\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmaino/Desktop/RLEM-seasonal-risk-index/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECE27E8-433E-4E91-85BF-A60D560F7C8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C12ED3C-A128-614B-961B-5E2F785E513B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59985B49-3727-4E83-A059-C008F5338E64}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26520" windowHeight="14600" xr2:uid="{59985B49-3727-4E83-A059-C008F5338E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Lentils/ chickpeas / canola</t>
   </si>
@@ -123,27 +123,9 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>Last year's crop</t>
-  </si>
-  <si>
-    <t>Last autumn</t>
-  </si>
-  <si>
-    <t>Last spring</t>
-  </si>
-  <si>
-    <t>This autumn</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Last year's cropping phase</t>
-  </si>
-  <si>
-    <t>This year</t>
-  </si>
-  <si>
     <t>Crop</t>
   </si>
   <si>
@@ -195,15 +177,9 @@
     <t>Heavy pasture canopy; minimal herbage removal (&gt; 2.8-4.0 t/ha) in Sept-Oct</t>
   </si>
   <si>
-    <t>Last year's pasture</t>
-  </si>
-  <si>
     <t>Pasture</t>
   </si>
   <si>
-    <t>Last year's pasture phase</t>
-  </si>
-  <si>
     <t>Crop type</t>
   </si>
   <si>
@@ -241,6 +217,27 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Upcoming rotation</t>
+  </si>
+  <si>
+    <t>Previous cropping rotation</t>
+  </si>
+  <si>
+    <t>Previous pasture rotation</t>
+  </si>
+  <si>
+    <t>Previous crop</t>
+  </si>
+  <si>
+    <t>Previous autumn</t>
+  </si>
+  <si>
+    <t>Previous spring</t>
+  </si>
+  <si>
+    <t>Upcoming autumn</t>
   </si>
 </sst>
 </file>
@@ -600,32 +597,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C28514-E217-4B09-8F84-134A3D686C22}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="64.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
         <v>27</v>
@@ -649,21 +646,21 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -684,21 +681,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -719,21 +716,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -754,21 +751,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -789,21 +786,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -824,21 +821,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -859,21 +856,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -894,135 +891,135 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G9">
         <v>-2</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G10">
         <v>-2</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G11">
         <v>-1</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G12">
         <v>-2</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1034,21 +1031,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
@@ -1069,56 +1066,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G14">
         <v>-2</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
@@ -1139,21 +1136,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D16">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
         <v>18</v>
@@ -1168,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K16">
         <v>3</v>

</xml_diff>